<commit_message>
update to a scraper to find relevant products
</commit_message>
<xml_diff>
--- a/ZORO/test_items.xlsx
+++ b/ZORO/test_items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Faha\random\walmart competitor scraper\new_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Faha\Projects\ZORO\zoro-repo\ZORO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92903AD-BD2D-48CB-BAFE-7A694004B38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FC602E-4D9F-4127-B6C2-87B7AE1157B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="1575" windowWidth="21600" windowHeight="11295" xr2:uid="{F03CD84B-0977-4D75-A868-10468539CC8E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F03CD84B-0977-4D75-A868-10468539CC8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>our_price</t>
   </si>
   <si>
-    <t>search_description</t>
-  </si>
-  <si>
     <t>Door locks</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Grade 2 Locks</t>
+  </si>
+  <si>
+    <t>Item Name</t>
   </si>
 </sst>
 </file>
@@ -485,15 +485,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="62" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,76 +500,76 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
-        <v>10</v>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="4">
         <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="4">
         <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="4">
         <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="4">
         <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big changes but still wip
</commit_message>
<xml_diff>
--- a/ZORO/test_items.xlsx
+++ b/ZORO/test_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Faha\Projects\ZORO\zoro-repo\ZORO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FC602E-4D9F-4127-B6C2-87B7AE1157B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B254ED-2521-4099-BB09-623D1834FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F03CD84B-0977-4D75-A868-10468539CC8E}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>DMR12</t>
   </si>
   <si>
-    <t>#12 Cotton Deck Mop Refill 8.1 oz.</t>
-  </si>
-  <si>
     <t>DMR16</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Item Name</t>
+  </si>
+  <si>
+    <t>Cotton Deck Mop Refill 8.1 oz.</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,13 +497,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,62 +514,62 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using ScrapingBee. Worked partially
</commit_message>
<xml_diff>
--- a/ZORO/test_items.xlsx
+++ b/ZORO/test_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Faha\Projects\ZORO\zoro-repo\ZORO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B254ED-2521-4099-BB09-623D1834FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6440EBF-6AC5-4AE0-B40E-BBAFD6CE65AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F03CD84B-0977-4D75-A868-10468539CC8E}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{F03CD84B-0977-4D75-A868-10468539CC8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Entry Lever Door Combo</t>
   </si>
   <si>
-    <t>Mortize locks</t>
-  </si>
-  <si>
     <t>Grade 3 Locks</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Cotton Deck Mop Refill 8.1 oz.</t>
+  </si>
+  <si>
+    <t>Mortise locks</t>
   </si>
 </sst>
 </file>
@@ -485,14 +485,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +504,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +559,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>